<commit_message>
cleaning up SFA exploration
</commit_message>
<xml_diff>
--- a/_projects/project2/zanudo2015_SFAexploration/classify_attractors/sfa/sfa_cluster_report.xlsx
+++ b/_projects/project2/zanudo2015_SFAexploration/classify_attractors/sfa/sfa_cluster_report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/ALS_IPS/zanudo2015/classify_attractors/sfa/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maddie/Documents/GitHub/CancerReversion/_projects/project2/zanudo2015_SFAexploration/classify_attractors/sfa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1776599F-56AF-0E48-897E-152FBFC535CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550F3002-9703-3A45-B9ED-F7E9223DA29C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="2060" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{D7293BAA-D1FB-8B45-AE8F-1BBD39CA19C8}"/>
+    <workbookView xWindow="4180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{D7293BAA-D1FB-8B45-AE8F-1BBD39CA19C8}"/>
   </bookViews>
   <sheets>
     <sheet name="both_12" sheetId="2" r:id="rId1"/>
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{495887F7-2665-6B48-8A49-76755FF6B4FB}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -773,13 +773,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5A9594-D60F-1348-9B09-F039004F9A61}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView zoomScale="144" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="11" max="11" width="14.83203125" customWidth="1"/>
   </cols>

</xml_diff>